<commit_message>
added PowerBi for dashboarding and added categorization variables to help visualize data KPI counters started
</commit_message>
<xml_diff>
--- a/Input/Input_Simulador.xlsx
+++ b/Input/Input_Simulador.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1FE460-B7FE-49BF-8B34-CC067AD560F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DB5E15-5CA7-4E5C-993B-4E813A6D5E4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="3432" windowWidth="17280" windowHeight="9072" firstSheet="2" activeTab="2" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="3" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="CapacidadSanitaria1" sheetId="23" state="hidden" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="176">
   <si>
     <t>id</t>
   </si>
@@ -570,6 +570,21 @@
   <si>
     <t>Cantidad Aislamiento</t>
   </si>
+  <si>
+    <t>Region Mapa PBI</t>
+  </si>
+  <si>
+    <t>Ciudad de Buenos Aires, Argentina</t>
+  </si>
+  <si>
+    <t>Gran Buenos Aires, Argentina</t>
+  </si>
+  <si>
+    <t>Provincia Buenos Aires, Argentina</t>
+  </si>
+  <si>
+    <t>Provincia de Santiago del Estero, Argentina</t>
+  </si>
 </sst>
 </file>
 
@@ -1029,7 +1044,7 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1179,6 +1194,7 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
@@ -4907,8 +4923,8 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4976,10 +4992,10 @@
         <v>5708369</v>
       </c>
       <c r="D2">
-        <v>-34.607568200000003</v>
-      </c>
-      <c r="E2">
-        <v>-58.437089399999998</v>
+        <v>-36.319937000000003</v>
+      </c>
+      <c r="E2" s="89">
+        <v>-59.810867000000002</v>
       </c>
       <c r="F2">
         <f>78781-F3</f>
@@ -5019,10 +5035,10 @@
         <v>9916715</v>
       </c>
       <c r="D3">
-        <v>-34.607568200000003</v>
+        <v>-34.479410999999999</v>
       </c>
       <c r="E3">
-        <v>-58.437089399999998</v>
+        <v>-58.617597000000004</v>
       </c>
       <c r="F3">
         <f>2681-202</f>
@@ -5146,10 +5162,10 @@
         <v>2890151</v>
       </c>
       <c r="D6">
-        <v>-34.607568200000003</v>
+        <v>-35.604559999999999</v>
       </c>
       <c r="E6">
-        <v>-58.437089399999998</v>
+        <v>-50.739153000000002</v>
       </c>
       <c r="F6">
         <v>202</v>
@@ -6029,10 +6045,10 @@
     <tabColor theme="7"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
@@ -6040,10 +6056,11 @@
     <col min="1" max="1" width="28.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="12" customWidth="1"/>
     <col min="3" max="3" width="20.5546875" style="12" customWidth="1"/>
-    <col min="4" max="16384" width="14" style="12"/>
+    <col min="4" max="4" width="51.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="14" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4">
+    <row r="1" spans="1:4" ht="14.4">
       <c r="A1" s="18" t="s">
         <v>101</v>
       </c>
@@ -6053,8 +6070,11 @@
       <c r="C1" s="18" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.4">
+      <c r="D1" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.4">
       <c r="A2" s="17" t="s">
         <v>9</v>
       </c>
@@ -6064,8 +6084,12 @@
       <c r="C2" s="17" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.4">
+      <c r="D2" s="12" t="str">
+        <f>+_xlfn.CONCAT("Provincia ",A2,", Argentina")</f>
+        <v>Provincia Tucumán, Argentina</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.4">
       <c r="A3" s="17" t="s">
         <v>11</v>
       </c>
@@ -6075,8 +6099,12 @@
       <c r="C3" s="17" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="14.4">
+      <c r="D3" s="12" t="str">
+        <f>+_xlfn.CONCAT("Provincia ",A3,", Argentina")</f>
+        <v>Provincia Salta, Argentina</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.4">
       <c r="A4" s="17" t="s">
         <v>12</v>
       </c>
@@ -6086,8 +6114,12 @@
       <c r="C4" s="17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.4">
+      <c r="D4" s="12" t="str">
+        <f t="shared" ref="D4:D26" si="0">+_xlfn.CONCAT("Provincia ",A4,", Argentina")</f>
+        <v>Provincia Misiones, Argentina</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.4">
       <c r="A5" s="17" t="s">
         <v>13</v>
       </c>
@@ -6097,8 +6129,12 @@
       <c r="C5" s="17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="14.4">
+      <c r="D5" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Chaco, Argentina</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.4">
       <c r="A6" s="17" t="s">
         <v>14</v>
       </c>
@@ -6108,8 +6144,12 @@
       <c r="C6" s="17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.4">
+      <c r="D6" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Corrientes, Argentina</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.4">
       <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
@@ -6119,8 +6159,11 @@
       <c r="C7" s="17" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.4">
+      <c r="D7" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.4">
       <c r="A8" s="17" t="s">
         <v>17</v>
       </c>
@@ -6130,8 +6173,12 @@
       <c r="C8" s="17" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="14.4">
+      <c r="D8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Jujuy, Argentina</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.4">
       <c r="A9" s="17" t="s">
         <v>20</v>
       </c>
@@ -6141,8 +6188,12 @@
       <c r="C9" s="17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="14.4">
+      <c r="D9" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Formosa, Argentina</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.4">
       <c r="A10" s="17" t="s">
         <v>23</v>
       </c>
@@ -6152,8 +6203,12 @@
       <c r="C10" s="17" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="14.4">
+      <c r="D10" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Catamarca, Argentina</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.4">
       <c r="A11" s="17" t="s">
         <v>24</v>
       </c>
@@ -6163,8 +6218,12 @@
       <c r="C11" s="17" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="14.4">
+      <c r="D11" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia La Rioja, Argentina</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.4">
       <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
@@ -6174,8 +6233,12 @@
       <c r="C12" s="17" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="14.4">
+      <c r="D12" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Mendoza, Argentina</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.4">
       <c r="A13" s="17" t="s">
         <v>16</v>
       </c>
@@ -6185,8 +6248,12 @@
       <c r="C13" s="17" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="14.4">
+      <c r="D13" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia San Juan, Argentina</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.4">
       <c r="A14" s="17" t="s">
         <v>22</v>
       </c>
@@ -6196,8 +6263,12 @@
       <c r="C14" s="17" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="14.4">
+      <c r="D14" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia San Luis, Argentina</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.4">
       <c r="A15" s="17" t="s">
         <v>18</v>
       </c>
@@ -6207,8 +6278,12 @@
       <c r="C15" s="17" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="14.4">
+      <c r="D15" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Río Negro, Argentina</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.4">
       <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
@@ -6218,8 +6293,12 @@
       <c r="C16" s="17" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.4">
+      <c r="D16" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Neuquén, Argentina</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.4">
       <c r="A17" s="17" t="s">
         <v>21</v>
       </c>
@@ -6229,8 +6308,12 @@
       <c r="C17" s="17" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.4">
+      <c r="D17" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Chubut, Argentina</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.4">
       <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
@@ -6240,9 +6323,13 @@
       <c r="C18" s="17" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.4">
-      <c r="A19" s="17" t="s">
+      <c r="D18" s="12" t="str">
+        <f>+_xlfn.CONCAT("Provincia ",A18,", Argentina")</f>
+        <v>Provincia La Pampa, Argentina</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.4">
+      <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -6251,8 +6338,12 @@
       <c r="C19" s="17" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.4">
+      <c r="D19" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Santa Cruz, Argentina</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.4">
       <c r="A20" s="17" t="s">
         <v>27</v>
       </c>
@@ -6262,8 +6353,12 @@
       <c r="C20" s="17" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.4">
+      <c r="D20" s="12" t="str">
+        <f>+A20</f>
+        <v>Tierra del Fuego</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.4">
       <c r="A21" s="17" t="s">
         <v>89</v>
       </c>
@@ -6273,8 +6368,12 @@
       <c r="C21" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.4">
+      <c r="D21" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Córdoba, Argentina</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.4">
       <c r="A22" s="17" t="s">
         <v>6</v>
       </c>
@@ -6284,8 +6383,12 @@
       <c r="C22" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.4">
+      <c r="D22" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Santa Fe, Argentina</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.4">
       <c r="A23" s="17" t="s">
         <v>104</v>
       </c>
@@ -6295,8 +6398,12 @@
       <c r="C23" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.4">
+      <c r="D23" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>Provincia Entre Ríos, Argentina</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.4">
       <c r="A24" s="17" t="s">
         <v>7</v>
       </c>
@@ -6306,8 +6413,11 @@
       <c r="C24" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.4">
+      <c r="D24" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.4">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
@@ -6317,8 +6427,11 @@
       <c r="C25" s="17" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1">
+      <c r="D25" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
@@ -6327,6 +6440,9 @@
       </c>
       <c r="C26" s="17" t="s">
         <v>72</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added KPI measures fixed "visible on upper agent bug" automatized export process at the end of the simulation's run
</commit_message>
<xml_diff>
--- a/Input/Input_Simulador.xlsx
+++ b/Input/Input_Simulador.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DB5E15-5CA7-4E5C-993B-4E813A6D5E4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BA269D-4E8B-4A38-B038-5B40A1138E3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="3" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
@@ -583,7 +583,7 @@
     <t>Provincia Buenos Aires, Argentina</t>
   </si>
   <si>
-    <t>Provincia de Santiago del Estero, Argentina</t>
+    <t xml:space="preserve"> Santiago del Estero, Argentina</t>
   </si>
 </sst>
 </file>
@@ -1189,12 +1189,12 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
@@ -4994,7 +4994,7 @@
       <c r="D2">
         <v>-36.319937000000003</v>
       </c>
-      <c r="E2" s="89">
+      <c r="E2" s="86">
         <v>-59.810867000000002</v>
       </c>
       <c r="F2">
@@ -6048,7 +6048,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
@@ -6115,7 +6115,7 @@
         <v>85</v>
       </c>
       <c r="D4" s="12" t="str">
-        <f t="shared" ref="D4:D26" si="0">+_xlfn.CONCAT("Provincia ",A4,", Argentina")</f>
+        <f t="shared" ref="D4:D23" si="0">+_xlfn.CONCAT("Provincia ",A4,", Argentina")</f>
         <v>Provincia Misiones, Argentina</v>
       </c>
     </row>
@@ -69531,11 +69531,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="88"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="89"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="17" t="s">

</xml_diff>

<commit_message>
fixed Santiago del Estero's location in PBI Map
</commit_message>
<xml_diff>
--- a/Input/Input_Simulador.xlsx
+++ b/Input/Input_Simulador.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BA269D-4E8B-4A38-B038-5B40A1138E3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA469A37-776D-4D0A-85D2-89A8DA167845}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="3" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
@@ -583,7 +583,7 @@
     <t>Provincia Buenos Aires, Argentina</t>
   </si>
   <si>
-    <t xml:space="preserve"> Santiago del Estero, Argentina</t>
+    <t>Provincia de Santiago del Estero</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1044,7 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1195,6 +1195,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
@@ -6159,7 +6162,7 @@
       <c r="C7" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="90" t="s">
         <v>175</v>
       </c>
     </row>
@@ -6446,8 +6449,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" display="https://es.wikipedia.org/wiki/Provincia_de_Santiago_del_Estero" xr:uid="{1855972F-57B5-41F3-9C8A-7C1844AA8C5B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
advances in visualization and minor fixes
</commit_message>
<xml_diff>
--- a/Input/Input_Simulador.xlsx
+++ b/Input/Input_Simulador.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA469A37-776D-4D0A-85D2-89A8DA167845}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1F9933-4855-4238-AD5E-1D5151E09B24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="3" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Provincias" sheetId="1" r:id="rId3"/>
     <sheet name="Diccionario" sheetId="15" r:id="rId4"/>
     <sheet name="CapacidadSanitariaCamas" sheetId="27" state="hidden" r:id="rId5"/>
-    <sheet name="Capacidad Sanitaria" sheetId="12" state="hidden" r:id="rId6"/>
+    <sheet name="Capacidad Sanitaria" sheetId="12" r:id="rId6"/>
     <sheet name="Perfil Etário" sheetId="2" r:id="rId7"/>
     <sheet name="matrizOD" sheetId="3" r:id="rId8"/>
     <sheet name="TiposdeMovimientos" sheetId="14" r:id="rId9"/>
@@ -577,13 +577,13 @@
     <t>Ciudad de Buenos Aires, Argentina</t>
   </si>
   <si>
-    <t>Gran Buenos Aires, Argentina</t>
-  </si>
-  <si>
     <t>Provincia Buenos Aires, Argentina</t>
   </si>
   <si>
     <t>Provincia de Santiago del Estero</t>
+  </si>
+  <si>
+    <t>Greater Buenos Aires</t>
   </si>
 </sst>
 </file>
@@ -1190,14 +1190,14 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
@@ -3012,7 +3012,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A26"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4351,7 +4351,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -4494,7 +4494,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -4600,7 +4600,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="66">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -4927,7 +4927,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6162,8 +6162,8 @@
       <c r="C7" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="90" t="s">
-        <v>175</v>
+      <c r="D7" s="87" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4">
@@ -6430,8 +6430,8 @@
       <c r="C25" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>173</v>
+      <c r="D25" s="35" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
@@ -6445,15 +6445,16 @@
         <v>72</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" display="https://es.wikipedia.org/wiki/Provincia_de_Santiago_del_Estero" xr:uid="{1855972F-57B5-41F3-9C8A-7C1844AA8C5B}"/>
+    <hyperlink ref="D25" r:id="rId2" display="https://en.wikipedia.org/wiki/Greater_Buenos_Aires" xr:uid="{E18A1ECB-961A-4646-B9F2-86F1DE126A3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -6859,7 +6860,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
@@ -69537,11 +69538,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="89"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="90"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="17" t="s">

</xml_diff>

<commit_message>
Bug fixes and visualization advances
</commit_message>
<xml_diff>
--- a/Input/Input_Simulador.xlsx
+++ b/Input/Input_Simulador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1F9933-4855-4238-AD5E-1D5151E09B24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F79E10-273A-4D4B-9B56-F3CF7F321A06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="3" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="10" activeTab="14" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="CapacidadSanitaria1" sheetId="23" state="hidden" r:id="rId1"/>
@@ -3508,8 +3508,8 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4208,7 +4208,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -4350,8 +4350,8 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -6050,7 +6050,7 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
when we met i was but the learner,now i am the master
</commit_message>
<xml_diff>
--- a/Input/Input_Simulador.xlsx
+++ b/Input/Input_Simulador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F79E10-273A-4D4B-9B56-F3CF7F321A06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C01CDD-022D-4D20-B307-0CDB385DA903}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="10" activeTab="14" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="2" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="CapacidadSanitaria1" sheetId="23" state="hidden" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="178">
   <si>
     <t>id</t>
   </si>
@@ -322,9 +322,6 @@
     <t>Sur</t>
   </si>
   <si>
-    <t>PBA - Partidos del GBA</t>
-  </si>
-  <si>
     <t>Córdoba</t>
   </si>
   <si>
@@ -584,6 +581,15 @@
   </si>
   <si>
     <t>Greater Buenos Aires</t>
+  </si>
+  <si>
+    <t>CABA</t>
+  </si>
+  <si>
+    <t>Partidos del GBA</t>
+  </si>
+  <si>
+    <t>Provincia de BA</t>
   </si>
 </sst>
 </file>
@@ -1996,13 +2002,13 @@
         <v>72</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>1</v>
@@ -2011,7 +2017,7 @@
         <v>2</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2097,7 +2103,7 @@
         <v>Centro</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K10">
         <v>3308876</v>
@@ -2252,7 +2258,7 @@
         <v>Centro</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K15">
         <v>1235994</v>
@@ -2614,7 +2620,7 @@
         <v>85</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>72</v>
@@ -2676,7 +2682,7 @@
         <v>85</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>72</v>
@@ -3034,10 +3040,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3135,7 +3141,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="82" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="84">
         <v>3308876</v>
@@ -3171,7 +3177,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="84">
         <v>1235994</v>
@@ -3529,7 +3535,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>40</v>
@@ -3538,13 +3544,13 @@
         <v>41</v>
       </c>
       <c r="E1" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>107</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>108</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>42</v>
@@ -3558,10 +3564,10 @@
         <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>109</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>110</v>
       </c>
       <c r="D2" s="22">
         <v>0.17899999999999999</v>
@@ -3571,7 +3577,7 @@
       <c r="G2" s="22"/>
       <c r="H2" s="4"/>
       <c r="I2" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.8">
@@ -3579,10 +3585,10 @@
         <v>46</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="36" t="s">
         <v>112</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>113</v>
       </c>
       <c r="D3" s="6">
         <v>0.5</v>
@@ -3600,7 +3606,7 @@
         <v>47</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>48</v>
@@ -3618,13 +3624,13 @@
     </row>
     <row r="5" spans="1:9" ht="28.8">
       <c r="A5" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -3639,13 +3645,13 @@
     </row>
     <row r="6" spans="1:9" ht="28.8">
       <c r="A6" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -3663,10 +3669,10 @@
         <v>50</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" s="22">
         <v>0.3</v>
@@ -3681,13 +3687,13 @@
     </row>
     <row r="8" spans="1:9" ht="15.6">
       <c r="A8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>117</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>118</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -3705,10 +3711,10 @@
         <v>52</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" s="22"/>
       <c r="E9" s="22">
@@ -3721,21 +3727,21 @@
         <v>14</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8">
       <c r="A10" s="71" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>122</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>123</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>53</v>
@@ -3750,21 +3756,21 @@
         <v>41</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.8">
       <c r="A11" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="C11" s="26" t="s">
         <v>126</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>127</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="28">
@@ -3777,21 +3783,21 @@
         <v>41</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I11" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28.8">
       <c r="A12" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="26" t="s">
         <v>128</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>129</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="28">
@@ -3804,21 +3810,21 @@
         <v>19</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="43.2">
       <c r="A13" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>130</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>131</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22">
@@ -3827,7 +3833,7 @@
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>54</v>
@@ -3835,13 +3841,13 @@
     </row>
     <row r="14" spans="1:9" ht="43.2">
       <c r="A14" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>132</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>133</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -3852,7 +3858,7 @@
         <v>42</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>54</v>
@@ -3860,13 +3866,13 @@
     </row>
     <row r="15" spans="1:9" ht="28.8">
       <c r="A15" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>134</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>135</v>
       </c>
       <c r="D15" s="31"/>
       <c r="E15" s="31">
@@ -3879,21 +3885,21 @@
         <v>14</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I15" s="43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.6">
       <c r="A16" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="74" t="s">
         <v>136</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" s="74" t="s">
-        <v>137</v>
       </c>
       <c r="D16" s="75"/>
       <c r="E16" s="75">
@@ -3906,7 +3912,7 @@
         <v>9</v>
       </c>
       <c r="H16" s="75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I16" s="74" t="s">
         <v>54</v>
@@ -3929,7 +3935,7 @@
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
       <c r="E18" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="32"/>
@@ -3938,7 +3944,7 @@
     </row>
     <row r="19" spans="1:9" ht="18">
       <c r="A19" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
@@ -3951,10 +3957,10 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>141</v>
       </c>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
@@ -3967,7 +3973,7 @@
     <row r="21" spans="1:9">
       <c r="A21" s="32"/>
       <c r="B21" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
@@ -4099,24 +4105,24 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1">
       <c r="A1" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="C1" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="D1" s="47" t="s">
         <v>145</v>
-      </c>
-      <c r="D1" s="47" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>147</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>148</v>
       </c>
       <c r="C2" s="49">
         <v>64000000</v>
@@ -4129,10 +4135,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="52" t="s">
         <v>149</v>
-      </c>
-      <c r="B3" s="52" t="s">
-        <v>150</v>
       </c>
       <c r="C3" s="53">
         <v>1920000</v>
@@ -4145,10 +4151,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="55">
         <f>C3/C2</f>
@@ -4161,10 +4167,10 @@
     </row>
     <row r="5" spans="1:7" ht="29.4" thickBot="1">
       <c r="A5" s="57" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="58" t="s">
         <v>152</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>153</v>
       </c>
       <c r="C5" s="59">
         <f>C4/C7</f>
@@ -4178,7 +4184,7 @@
     <row r="6" spans="1:7" ht="15" thickBot="1"/>
     <row r="7" spans="1:7" ht="15" thickBot="1">
       <c r="A7" s="61" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B7" s="46"/>
       <c r="C7" s="47">
@@ -4226,7 +4232,7 @@
         <v>63</v>
       </c>
       <c r="C1" s="62" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4350,7 +4356,7 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -4369,7 +4375,7 @@
         <v>63</v>
       </c>
       <c r="C1" s="62" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4642,7 +4648,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4744,7 +4750,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="64" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4854,15 +4860,15 @@
         <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="80" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4907,7 +4913,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9">
         <v>193739</v>
@@ -4926,8 +4932,8 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5015,7 +5021,7 @@
         <v>1000</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="64">
         <v>31049</v>
@@ -5075,7 +5081,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4">
         <v>3308876</v>
@@ -5184,7 +5190,7 @@
         <v>500</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" s="64">
         <v>15720</v>
@@ -5285,7 +5291,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9">
         <v>1235994</v>
@@ -5436,7 +5442,7 @@
         <v>10</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="64">
         <v>3176</v>
@@ -6051,7 +6057,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>
@@ -6065,16 +6071,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="14.4">
       <c r="A1" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>103</v>
-      </c>
       <c r="D1" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.4">
@@ -6082,7 +6088,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>86</v>
@@ -6097,7 +6103,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>86</v>
@@ -6112,7 +6118,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>85</v>
@@ -6127,7 +6133,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>85</v>
@@ -6142,7 +6148,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>85</v>
@@ -6157,13 +6163,13 @@
         <v>15</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>86</v>
       </c>
       <c r="D7" s="87" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4">
@@ -6171,7 +6177,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>86</v>
@@ -6186,7 +6192,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>85</v>
@@ -6201,7 +6207,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>86</v>
@@ -6216,7 +6222,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>86</v>
@@ -6276,7 +6282,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>87</v>
@@ -6291,7 +6297,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>87</v>
@@ -6306,7 +6312,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>87</v>
@@ -6321,7 +6327,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>87</v>
@@ -6336,7 +6342,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>87</v>
@@ -6351,7 +6357,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>87</v>
@@ -6363,10 +6369,10 @@
     </row>
     <row r="21" spans="1:4" ht="14.4">
       <c r="A21" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>72</v>
@@ -6381,7 +6387,7 @@
         <v>6</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>72</v>
@@ -6393,10 +6399,10 @@
     </row>
     <row r="23" spans="1:4" ht="14.4">
       <c r="A23" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>72</v>
@@ -6411,13 +6417,13 @@
         <v>7</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.4">
@@ -6425,13 +6431,13 @@
         <v>31</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>88</v>
+        <v>176</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>72</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
@@ -6439,13 +6445,13 @@
         <v>32</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>72</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -6475,13 +6481,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="77" t="s">
         <v>169</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>170</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -6517,7 +6523,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="76" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="64">
         <v>710</v>
@@ -6587,7 +6593,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="64">
         <v>265</v>
@@ -69539,25 +69545,25 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="88" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="89"/>
       <c r="C1" s="90"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="20">
         <v>53.7</v>
@@ -69568,7 +69574,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="20">
         <v>41.2</v>
@@ -69579,7 +69585,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="20">
         <v>2.2000000000000002</v>
@@ -69590,7 +69596,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="20">
         <v>2.9</v>

</xml_diff>

<commit_message>
rework of 'enfermo' statechart -> the asymptomatic state includes the incubation period as it is defined as the period before the first symptoms. Changes according to the new statechart done in pbi
</commit_message>
<xml_diff>
--- a/Input/Input_Simulador.xlsx
+++ b/Input/Input_Simulador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C01CDD-022D-4D20-B307-0CDB385DA903}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BEA907-9530-475C-8D43-045AA39A5856}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="2" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="3" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="CapacidadSanitaria1" sheetId="23" state="hidden" r:id="rId1"/>
@@ -4932,8 +4932,8 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5021,7 +5021,7 @@
         <v>1000</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="64">
         <v>31049</v>
@@ -5064,7 +5064,7 @@
         <v>1000</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="64">
         <v>53940</v>
@@ -5190,7 +5190,7 @@
         <v>500</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6" s="64">
         <v>15720</v>
@@ -5442,7 +5442,7 @@
         <v>10</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="64">
         <v>3176</v>
@@ -6056,8 +6056,8 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" customHeight="1"/>

</xml_diff>